<commit_message>
All adjustments have been implemented
Bugs have been taken care of
</commit_message>
<xml_diff>
--- a/GenerateYearlyReportPerformer/Data/Config.xlsx
+++ b/GenerateYearlyReportPerformer/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adyma\Documents\UiPath\Aplicatii\GenerateYearlyReportPerformer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adyma\Documents\GitHub\GenerateYearlyReport\GenerateYearlyReportPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3138075-30A2-446E-BEB3-F711E5C05DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C60B667-060A-4EDB-8C0F-44F11351736E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -143,6 +143,15 @@
   </si>
   <si>
     <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>ReportsDownloadPath</t>
+  </si>
+  <si>
+    <t>\ReportsDownloadPath</t>
+  </si>
+  <si>
+    <t>inYear</t>
   </si>
 </sst>
 </file>
@@ -529,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -609,39 +618,53 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <v>2020</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="C14" s="5"/>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="C16" s="5"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="3:3" ht="14.25" customHeight="1">
+      <c r="C18" s="5"/>
     </row>
-    <row r="17" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="18" spans="3:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="3:3" ht="14.25" customHeight="1">
-      <c r="C20" s="5"/>
+    <row r="20" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="3:3" ht="14.25" customHeight="1">
+      <c r="C21" s="5"/>
     </row>
-    <row r="21" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="3:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="3:3" ht="14.25" customHeight="1">
-      <c r="C23" s="5"/>
+    <row r="22" spans="3:3" ht="14.25" customHeight="1">
+      <c r="C22" s="5"/>
     </row>
-    <row r="24" spans="3:3" ht="14.25" customHeight="1">
-      <c r="C24" s="5"/>
-    </row>
+    <row r="23" spans="3:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="3:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="3:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="3:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="3:3" ht="14.25" customHeight="1"/>
@@ -1613,8 +1636,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1626,7 +1647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>